<commit_message>
Add more analysis for selected tasks
Signed-off-by: Liang Zhang <psychelzh@outlook.com>
</commit_message>
<xml_diff>
--- a/posts/prepare-training/candidates.xlsx
+++ b/posts/prepare-training/candidates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e24742936e72e2bc/Documents/Research/cogstruct-dev/posts/prepare-training/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{50E3E9C2-4E3B-42E7-9295-A2A3089FABEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8396C10B-2687-4FE1-85E1-8E5A47E30976}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{50E3E9C2-4E3B-42E7-9295-A2A3089FABEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7B7804A-A8F1-4DE9-8924-345D9F4D6C23}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{42EC2D2F-19B4-4732-AE8F-F23D586C7B58}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>舒尔特方格（中级）</t>
   </si>
@@ -52,9 +52,6 @@
     <t>超级秒表PRO</t>
   </si>
   <si>
-    <t>密码箱</t>
-  </si>
-  <si>
     <t>幸运小球</t>
   </si>
   <si>
@@ -64,18 +61,6 @@
     <t>蝴蝶照相机</t>
   </si>
   <si>
-    <t>顺背数PRO</t>
-  </si>
-  <si>
-    <t>倒背数PRO</t>
-  </si>
-  <si>
-    <t>文字卡片</t>
-  </si>
-  <si>
-    <t>美术卡片</t>
-  </si>
-  <si>
     <t>图形推理</t>
   </si>
   <si>
@@ -104,6 +89,34 @@
   </si>
   <si>
     <t>瑞文高级推理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宇宙黑洞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时空相机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>general</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置记忆PRO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>格子卡片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数字卡片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>速算师（中级）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -468,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB557001-62EA-4014-B3EC-2702073E5D44}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -481,10 +494,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -492,7 +505,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -500,7 +513,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -508,7 +521,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -516,7 +529,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -524,87 +537,95 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
         <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>